<commit_message>
Log sheet written up and gantt chart updated.
</commit_message>
<xml_diff>
--- a/docs/logs/Gantt_chart.xlsx
+++ b/docs/logs/Gantt_chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="13395" windowHeight="6975" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="13395" windowHeight="6975"/>
   </bookViews>
   <sheets>
     <sheet name="Gannt Data" sheetId="3" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Task</t>
   </si>
@@ -23,9 +23,6 @@
     <t>Start</t>
   </si>
   <si>
-    <t>Duration</t>
-  </si>
-  <si>
     <t>Merge/Set up Repositories</t>
   </si>
   <si>
@@ -93,6 +90,45 @@
   </si>
   <si>
     <t>Days from Demo Date to Now:</t>
+  </si>
+  <si>
+    <t>Completion Day</t>
+  </si>
+  <si>
+    <t>Estimated Days To Complete</t>
+  </si>
+  <si>
+    <t>Target Completion Date</t>
+  </si>
+  <si>
+    <t>Date Completed</t>
+  </si>
+  <si>
+    <t>Assigned Team Member</t>
+  </si>
+  <si>
+    <t>Hamzah</t>
+  </si>
+  <si>
+    <t>Eiran</t>
+  </si>
+  <si>
+    <t>Horatio</t>
+  </si>
+  <si>
+    <t>Michal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t>Estimated Hours To Complete</t>
+  </si>
+  <si>
+    <t>Duration Days</t>
+  </si>
+  <si>
+    <t>Duration Hours</t>
   </si>
 </sst>
 </file>
@@ -124,7 +160,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -132,11 +168,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -144,6 +189,12 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,7 +396,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Duration</c:v>
+                  <c:v>Duration Days</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -481,11 +532,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="38594048"/>
-        <c:axId val="38606336"/>
+        <c:axId val="100258944"/>
+        <c:axId val="100260864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="38594048"/>
+        <c:axId val="100258944"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -519,7 +570,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38606336"/>
+        <c:crossAx val="100260864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -527,7 +578,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38606336"/>
+        <c:axId val="100260864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="28"/>
@@ -559,7 +610,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="38594048"/>
+        <c:crossAx val="100258944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -901,19 +952,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -921,12 +981,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -935,13 +1016,36 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D10" si="0">SUM(B2:C2)</f>
+        <f>C2*24</f>
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E10" si="0">SUM(B2:C2)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" t="str">
+        <f>CONCATENATE($A$31,$C$31,$A$32)</f>
+        <v>951926, 1024072</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <f>H2*24</f>
+        <v>12</v>
+      </c>
+      <c r="J2" s="3">
+        <f>B2+H2+$A$22</f>
+        <v>41229.5</v>
+      </c>
+      <c r="K2" s="3">
+        <f>$A$22+E2</f>
+        <v>41230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -950,13 +1054,36 @@
         <v>1</v>
       </c>
       <c r="D3">
+        <f t="shared" ref="D3:D18" si="1">C3*24</f>
+        <v>24</v>
+      </c>
+      <c r="E3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" t="str">
+        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
+        <v>951926, 1024072, 1001231, 1028907</v>
+      </c>
+      <c r="H3">
+        <v>0.5</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I18" si="2">H3*24</f>
+        <v>12</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J18" si="3">B3+H3+$A$22</f>
+        <v>41229.5</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K18" si="4">$A$22+E3</f>
+        <v>41230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -965,13 +1092,36 @@
         <v>1</v>
       </c>
       <c r="D4">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="E4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" t="str">
+        <f>CONCATENATE($A$31,$C$31,$A$32)</f>
+        <v>951926, 1024072</v>
+      </c>
+      <c r="H4">
+        <v>0.5</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="3"/>
+        <v>41229.5</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="4"/>
+        <v>41230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -980,13 +1130,36 @@
         <v>2</v>
       </c>
       <c r="D5">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="E5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" t="str">
+        <f>CONCATENATE($A$33,$C$31,$A$34)</f>
+        <v>1001231, 1028907</v>
+      </c>
+      <c r="H5">
+        <v>0.25</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="3"/>
+        <v>41229.25</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="4"/>
+        <v>41231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -995,13 +1168,36 @@
         <v>3</v>
       </c>
       <c r="D6">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="E6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" t="str">
+        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
+        <v>951926, 1024072, 1001231, 1028907</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="3"/>
+        <v>41232</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="4"/>
+        <v>41234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1010,13 +1206,36 @@
         <v>1</v>
       </c>
       <c r="D7">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" t="str">
+        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
+        <v>951926, 1024072, 1001231, 1028907</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="3"/>
+        <v>41234</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="4"/>
+        <v>41234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -1025,13 +1244,36 @@
         <v>0.5</v>
       </c>
       <c r="D8">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" t="str">
+        <f>CONCATENATE($A$31,$C$31,$A$32)</f>
+        <v>951926, 1024072</v>
+      </c>
+      <c r="H8">
+        <v>0.5</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="3"/>
+        <v>41234.5</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="4"/>
+        <v>41234.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -1040,13 +1282,36 @@
         <v>1</v>
       </c>
       <c r="D9">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" t="str">
+        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
+        <v>951926, 1024072, 1001231, 1028907</v>
+      </c>
+      <c r="H9">
+        <v>0.25</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="3"/>
+        <v>41234.25</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="4"/>
+        <v>41235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -1055,13 +1320,36 @@
         <v>7</v>
       </c>
       <c r="D10">
+        <f t="shared" si="1"/>
+        <v>168</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" t="str">
+        <f>CONCATENATE($A$33,$C$31,$A$34)</f>
+        <v>1001231, 1028907</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="3"/>
+        <v>41237</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="4"/>
+        <v>41242</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -1070,13 +1358,36 @@
         <v>4</v>
       </c>
       <c r="D11">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="E11">
         <f>SUM(B11:C11)</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11" t="str">
+        <f>CONCATENATE($A$33,$C$31,$A$34)</f>
+        <v>1001231, 1028907</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="3"/>
+        <v>41239</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="4"/>
+        <v>41242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -1085,13 +1396,36 @@
         <v>14</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:D17" si="1">SUM(B12:C12)</f>
+        <f t="shared" si="1"/>
+        <v>336</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:E17" si="5">SUM(B12:C12)</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" t="str">
+        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
+        <v>951926, 1024072, 1001231, 1028907</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="3"/>
+        <v>41240</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="4"/>
+        <v>41249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>13</v>
@@ -1101,12 +1435,35 @@
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" t="str">
+        <f>CONCATENATE($A$33,$C$31,$A$34)</f>
+        <v>1001231, 1028907</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="3"/>
+        <v>41243</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="4"/>
+        <v>41244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>15</v>
@@ -1116,12 +1473,35 @@
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="E14">
+        <f>SUM(B14:C14)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G14" t="str">
+        <f>CONCATENATE($A$33,$C$31,$A$34)</f>
+        <v>1001231, 1028907</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="3"/>
+        <v>41245</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="4"/>
+        <v>41245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>16</v>
@@ -1131,34 +1511,73 @@
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="E15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16">
+      <c r="G15" t="str">
+        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
+        <v>951926, 1024072, 1001231, 1028907</v>
+      </c>
+      <c r="H15">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="3"/>
+        <v>41245.083333333336</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="4"/>
+        <v>41246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5">
         <v>15</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="5">
         <v>3</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="5">
         <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
-      <c r="E16">
-        <f>MAX(D2:D16)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G16" s="5" t="str">
+        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
+        <v>951926, 1024072, 1001231, 1028907</v>
+      </c>
+      <c r="H16" s="5">
+        <v>3</v>
+      </c>
+      <c r="I16" s="5">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="J16" s="10">
+        <f t="shared" si="3"/>
+        <v>41247</v>
+      </c>
+      <c r="K16" s="10">
+        <f t="shared" si="4"/>
+        <v>41247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>20</v>
@@ -1168,12 +1587,35 @@
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
+        <v>192</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G17" s="8" t="str">
+        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
+        <v>951926, 1024072, 1001231, 1028907</v>
+      </c>
+      <c r="H17" s="9">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="3"/>
+        <v>41254</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="4"/>
+        <v>41257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>21</v>
@@ -1182,22 +1624,48 @@
         <v>2</v>
       </c>
       <c r="D18">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="E18">
         <f>SUM(B18:C18)</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G18" t="str">
+        <f>CONCATENATE($A$34)</f>
+        <v>1028907</v>
+      </c>
+      <c r="H18" s="9">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="J18" s="3">
+        <f t="shared" si="3"/>
+        <v>41252</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" si="4"/>
+        <v>41252</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>41229</v>
       </c>
@@ -1208,16 +1676,24 @@
         <f>B22-A22</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f>MAX(E2:E16)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>41281</v>
       </c>
@@ -1226,8 +1702,48 @@
         <v>32</v>
       </c>
     </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>951926</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>1024072</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>1001231</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>1028907</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1235,7 +1751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Log sheet and gantt chart updated
</commit_message>
<xml_diff>
--- a/docs/logs/Gantt_chart.xlsx
+++ b/docs/logs/Gantt_chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="13395" windowHeight="6975"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="13395" windowHeight="6975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Gannt Data" sheetId="3" r:id="rId1"/>
@@ -15,23 +15,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Task</t>
   </si>
   <si>
-    <t>Start</t>
-  </si>
-  <si>
     <t>Merge/Set up Repositories</t>
   </si>
   <si>
-    <t>Create launch file for webcam</t>
-  </si>
-  <si>
-    <t>Install OpenCV</t>
-  </si>
-  <si>
     <t>Understand Kinect Data</t>
   </si>
   <si>
@@ -83,21 +74,12 @@
     <t>Report Outline</t>
   </si>
   <si>
-    <t>Days taken to complete programming:</t>
-  </si>
-  <si>
     <t>Today:</t>
   </si>
   <si>
     <t>Days from Demo Date to Now:</t>
   </si>
   <si>
-    <t>Completion Day</t>
-  </si>
-  <si>
-    <t>Estimated Days To Complete</t>
-  </si>
-  <si>
     <t>Target Completion Date</t>
   </si>
   <si>
@@ -129,6 +111,15 @@
   </si>
   <si>
     <t>Duration Hours</t>
+  </si>
+  <si>
+    <t>Setup Webcam</t>
+  </si>
+  <si>
+    <t>Install &amp; Setup OpenCV</t>
+  </si>
+  <si>
+    <t>Start Day</t>
   </si>
 </sst>
 </file>
@@ -181,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -191,9 +182,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -258,7 +247,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Start</c:v>
+                  <c:v>Start Day</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -279,10 +268,10 @@
                   <c:v>Initial Discussion</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Create launch file for webcam</c:v>
+                  <c:v>Setup Webcam</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Install OpenCV</c:v>
+                  <c:v>Install &amp; Setup OpenCV</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Implementing CV Bridge Node</c:v>
@@ -339,10 +328,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
@@ -388,11 +377,11 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Gannt Data'!$C$1</c:f>
+              <c:f>'Gannt Data'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -414,10 +403,10 @@
                   <c:v>Initial Discussion</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Create launch file for webcam</c:v>
+                  <c:v>Setup Webcam</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Install OpenCV</c:v>
+                  <c:v>Install &amp; Setup OpenCV</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Implementing CV Bridge Node</c:v>
@@ -463,7 +452,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gannt Data'!$C$2:$C$18</c:f>
+              <c:f>'Gannt Data'!$D$2:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -480,40 +469,40 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2</c:v>
@@ -581,7 +570,7 @@
         <c:axId val="100260864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="28"/>
+          <c:max val="30"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -613,7 +602,6 @@
         <c:crossAx val="100258944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -952,720 +940,572 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <f>ROUNDUP(C2/6,0)</f>
         <v>1</v>
       </c>
-      <c r="D2">
-        <f>C2*24</f>
-        <v>24</v>
-      </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E10" si="0">SUM(B2:C2)</f>
-        <v>1</v>
-      </c>
-      <c r="G2" t="str">
-        <f>CONCATENATE($A$31,$C$31,$A$32)</f>
+      <c r="E2" t="str">
+        <f>CONCATENATE($A$31,$B$35,$A$32)</f>
         <v>951926, 1024072</v>
       </c>
-      <c r="H2">
-        <v>0.5</v>
-      </c>
-      <c r="I2">
-        <f>H2*24</f>
-        <v>12</v>
-      </c>
-      <c r="J2" s="3">
-        <f>B2+H2+$A$22</f>
-        <v>41229.5</v>
-      </c>
-      <c r="K2" s="3">
-        <f>$A$22+E2</f>
-        <v>41230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3">
+        <f>B2+(F2/24)+$A$22</f>
+        <v>41229.083333333336</v>
+      </c>
+      <c r="H2" s="3">
+        <f>$A$22+B2+(C2/24)</f>
+        <v>41229.125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <f>ROUNDUP(C3/6,0)</f>
         <v>1</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D18" si="1">C3*24</f>
-        <v>24</v>
-      </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
+      <c r="E3" t="str">
+        <f>CONCATENATE($A$31,$B$35,$A$32,$B$35,$A$33,$B$35,$A$34)</f>
+        <v>951926, 1024072, 1001231, 1028907</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3">
+        <f>B3+(F3/24)+$A$22</f>
+        <v>41229.125</v>
+      </c>
+      <c r="H3" s="3">
+        <f>$A$22+B3+(C3/24)</f>
+        <v>41229.166666666664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="G3" t="str">
-        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
-        <v>951926, 1024072, 1001231, 1028907</v>
-      </c>
-      <c r="H3">
-        <v>0.5</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I18" si="2">H3*24</f>
-        <v>12</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" ref="J3:J18" si="3">B3+H3+$A$22</f>
-        <v>41229.5</v>
-      </c>
-      <c r="K3" s="3">
-        <f t="shared" ref="K3:K18" si="4">$A$22+E3</f>
-        <v>41230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <f>ROUNDUP(C4/6,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E4" t="str">
+        <f>CONCATENATE($A$31,$B$35,$A$32)</f>
+        <v>951926, 1024072</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
+      <c r="G4" s="3">
+        <f>B4+(F4/24)+$A$22</f>
+        <v>41230.125</v>
+      </c>
+      <c r="H4" s="3">
+        <f>$A$22+B4+(C4/24)</f>
+        <v>41230.208333333336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G4" t="str">
-        <f>CONCATENATE($A$31,$C$31,$A$32)</f>
-        <v>951926, 1024072</v>
-      </c>
-      <c r="H4">
-        <v>0.5</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="J4" s="3">
-        <f t="shared" si="3"/>
-        <v>41229.5</v>
-      </c>
-      <c r="K4" s="3">
-        <f t="shared" si="4"/>
-        <v>41230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
       <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <f>ROUNDUP(C5/6,0)</f>
         <v>2</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G5" t="str">
-        <f>CONCATENATE($A$33,$C$31,$A$34)</f>
+      <c r="E5" t="str">
+        <f>CONCATENATE($A$33,$B$35,$A$34)</f>
         <v>1001231, 1028907</v>
       </c>
-      <c r="H5">
-        <v>0.25</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="J5" s="3">
-        <f t="shared" si="3"/>
-        <v>41229.25</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" si="4"/>
-        <v>41231</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>1.5</v>
+      </c>
+      <c r="G5" s="3">
+        <f>B5+(F5/24)+$A$22</f>
+        <v>41230.0625</v>
+      </c>
+      <c r="H5" s="3">
+        <f>$A$22+B5+(C5/24)</f>
+        <v>41230.333333333336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G6" t="str">
-        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
+        <f>ROUNDUP(C6/6,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E6" t="str">
+        <f>CONCATENATE($A$31,$B$35,$A$32,$B$35,$A$33,$B$35,$A$34)</f>
         <v>951926, 1024072, 1001231, 1028907</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="J6" s="3">
-        <f t="shared" si="3"/>
-        <v>41232</v>
-      </c>
-      <c r="K6" s="3">
-        <f t="shared" si="4"/>
-        <v>41234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6" s="3">
+        <f>B6+(F6/24)+$A$22</f>
+        <v>41231.25</v>
+      </c>
+      <c r="H6" s="3">
+        <f>$A$22+B6+(C6/24)</f>
+        <v>41231.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <f>ROUNDUP(C7/6,0)</f>
         <v>1</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G7" t="str">
-        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
+      <c r="E7" t="str">
+        <f>CONCATENATE($A$31,$B$35,$A$32,$B$35,$A$33,$B$35,$A$34)</f>
         <v>951926, 1024072, 1001231, 1028907</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="J7" s="3">
-        <f t="shared" si="3"/>
-        <v>41234</v>
-      </c>
-      <c r="K7" s="3">
-        <f t="shared" si="4"/>
-        <v>41234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" s="3">
+        <f>B7+(F7/24)+$A$22</f>
+        <v>41233.25</v>
+      </c>
+      <c r="H7" s="3">
+        <f>$A$22+B7+(C7/24)</f>
+        <v>41233.166666666664</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>5</v>
       </c>
       <c r="C8">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>5.5</v>
-      </c>
-      <c r="G8" t="str">
-        <f>CONCATENATE($A$31,$C$31,$A$32)</f>
+        <f>ROUNDUP(C8/6,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E8" t="str">
+        <f>CONCATENATE($A$31,$B$35,$A$32)</f>
         <v>951926, 1024072</v>
       </c>
-      <c r="H8">
-        <v>0.5</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="J8" s="3">
-        <f t="shared" si="3"/>
-        <v>41234.5</v>
-      </c>
-      <c r="K8" s="3">
-        <f t="shared" si="4"/>
-        <v>41234.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3">
+        <f>B8+(F8/24)+$A$22</f>
+        <v>41234.125</v>
+      </c>
+      <c r="H8" s="3">
+        <f>$A$22+B8+(C8/24)</f>
+        <v>41234.083333333336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>5</v>
       </c>
       <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <f>ROUNDUP(C9/6,0)</f>
         <v>1</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
+      <c r="E9" t="str">
+        <f>CONCATENATE($A$31,$B$35,$A$32,$B$35,$A$33,$B$35,$A$34)</f>
+        <v>951926, 1024072, 1001231, 1028907</v>
+      </c>
+      <c r="F9">
+        <v>1.5</v>
+      </c>
+      <c r="G9" s="3">
+        <f>B9+(F9/24)+$A$22</f>
+        <v>41234.0625</v>
+      </c>
+      <c r="H9" s="3">
+        <f>$A$22+B9+(C9/24)</f>
+        <v>41234.166666666664</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
-      </c>
-      <c r="G9" t="str">
-        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
-        <v>951926, 1024072, 1001231, 1028907</v>
-      </c>
-      <c r="H9">
-        <v>0.25</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="3"/>
-        <v>41234.25</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" si="4"/>
-        <v>41235</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
       </c>
       <c r="B10">
         <v>6</v>
       </c>
       <c r="C10">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
-        <v>168</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="G10" t="str">
-        <f>CONCATENATE($A$33,$C$31,$A$34)</f>
+        <f>ROUNDUP(C10/6,0)</f>
+        <v>10</v>
+      </c>
+      <c r="E10" t="str">
+        <f>CONCATENATE($A$33,$B$35,$A$34)</f>
         <v>1001231, 1028907</v>
       </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-      <c r="J10" s="3">
-        <f t="shared" si="3"/>
-        <v>41237</v>
-      </c>
-      <c r="K10" s="3">
-        <f t="shared" si="4"/>
-        <v>41242</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>12</v>
+      </c>
+      <c r="G10" s="3">
+        <f>B10+(F10/24)+$A$22</f>
+        <v>41235.5</v>
+      </c>
+      <c r="H10" s="3">
+        <f>$A$22+B10+(C10/24)</f>
+        <v>41237.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="E11">
-        <f>SUM(B11:C11)</f>
-        <v>13</v>
-      </c>
-      <c r="G11" t="str">
-        <f>CONCATENATE($A$33,$C$31,$A$34)</f>
+        <f>ROUNDUP(C11/6,0)</f>
+        <v>3</v>
+      </c>
+      <c r="E11" t="str">
+        <f>CONCATENATE($A$33,$B$35,$A$34)</f>
         <v>1001231, 1028907</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="J11" s="3">
-        <f t="shared" si="3"/>
-        <v>41239</v>
-      </c>
-      <c r="K11" s="3">
-        <f t="shared" si="4"/>
-        <v>41242</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11" s="3">
+        <f>B11+(F11/24)+$A$22</f>
+        <v>41238.25</v>
+      </c>
+      <c r="H11" s="3">
+        <f>$A$22+B11+(C11/24)</f>
+        <v>41238.666666666664</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B12">
         <v>6</v>
       </c>
       <c r="C12">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
-        <v>336</v>
-      </c>
-      <c r="E12">
-        <f t="shared" ref="E12:E17" si="5">SUM(B12:C12)</f>
-        <v>20</v>
-      </c>
-      <c r="G12" t="str">
-        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
+        <f>ROUNDUP(C12/6,0)</f>
+        <v>10</v>
+      </c>
+      <c r="E12" t="str">
+        <f>CONCATENATE($A$31,$B$35,$A$32,$B$35,$A$33,$B$35,$A$34)</f>
         <v>951926, 1024072, 1001231, 1028907</v>
       </c>
-      <c r="H12">
-        <v>5</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="2"/>
-        <v>120</v>
-      </c>
-      <c r="J12" s="3">
-        <f t="shared" si="3"/>
-        <v>41240</v>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" si="4"/>
-        <v>41249</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>30</v>
+      </c>
+      <c r="G12" s="3">
+        <f>B12+(F12/24)+$A$22</f>
+        <v>41236.25</v>
+      </c>
+      <c r="H12" s="3">
+        <f>$A$22+B12+(C12/24)</f>
+        <v>41237.333333333336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>13</v>
       </c>
       <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <f>ROUNDUP(C13/6,0)</f>
         <v>2</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
-      <c r="G13" t="str">
-        <f>CONCATENATE($A$33,$C$31,$A$34)</f>
+      <c r="E13" t="str">
+        <f>CONCATENATE($A$33,$B$35,$A$34)</f>
         <v>1001231, 1028907</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="J13" s="3">
-        <f t="shared" si="3"/>
-        <v>41243</v>
-      </c>
-      <c r="K13" s="3">
-        <f t="shared" si="4"/>
-        <v>41244</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13" s="3">
+        <f>B13+(F13/24)+$A$22</f>
+        <v>41242.25</v>
+      </c>
+      <c r="H13" s="3">
+        <f>$A$22+B13+(C13/24)</f>
+        <v>41242.333333333336</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>15</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="E14">
-        <f>SUM(B14:C14)</f>
-        <v>16</v>
-      </c>
-      <c r="G14" t="str">
-        <f>CONCATENATE($A$33,$C$31,$A$34)</f>
+        <f>ROUNDUP(C14/6,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E14" t="str">
+        <f>CONCATENATE($A$33,$B$35,$A$34)</f>
         <v>1001231, 1028907</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="J14" s="3">
-        <f t="shared" si="3"/>
-        <v>41245</v>
-      </c>
-      <c r="K14" s="3">
-        <f t="shared" si="4"/>
-        <v>41245</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14" s="3">
+        <f>B14+(F14/24)+$A$22</f>
+        <v>41244.25</v>
+      </c>
+      <c r="H14" s="3">
+        <f>$A$22+B14+(C14/24)</f>
+        <v>41244.416666666664</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <v>16</v>
       </c>
       <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <f>ROUNDUP(C15/6,0)</f>
         <v>1</v>
       </c>
-      <c r="D15">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-      <c r="G15" t="str">
-        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
+      <c r="E15" t="str">
+        <f>CONCATENATE($A$31,$B$35,$A$32,$B$35,$A$33,$B$35,$A$34)</f>
         <v>951926, 1024072, 1001231, 1028907</v>
       </c>
-      <c r="H15">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J15" s="3">
-        <f t="shared" si="3"/>
-        <v>41245.083333333336</v>
-      </c>
-      <c r="K15" s="3">
-        <f t="shared" si="4"/>
-        <v>41246</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="3">
+        <f>B15+(F15/24)+$A$22</f>
+        <v>41245.020833333336</v>
+      </c>
+      <c r="H15" s="3">
+        <f>$A$22+B15+(C15/24)</f>
+        <v>41245.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B16" s="5">
         <v>15</v>
       </c>
       <c r="C16" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D16" s="5">
-        <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="E16" s="5">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(C16/6,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E16" s="5" t="str">
+        <f>CONCATENATE($A$31,$B$35,$A$32,$B$35,$A$33,$B$35,$A$34)</f>
+        <v>951926, 1024072, 1001231, 1028907</v>
+      </c>
+      <c r="F16" s="5">
         <v>18</v>
       </c>
-      <c r="G16" s="5" t="str">
-        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
-        <v>951926, 1024072, 1001231, 1028907</v>
-      </c>
-      <c r="H16" s="5">
-        <v>3</v>
-      </c>
-      <c r="I16" s="5">
-        <f t="shared" si="2"/>
-        <v>72</v>
-      </c>
-      <c r="J16" s="10">
-        <f t="shared" si="3"/>
-        <v>41247</v>
-      </c>
-      <c r="K16" s="10">
-        <f t="shared" si="4"/>
-        <v>41247</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G16" s="8">
+        <f>B16+(F16/24)+$A$22</f>
+        <v>41244.75</v>
+      </c>
+      <c r="H16" s="8">
+        <f>$A$22+B16+(C16/24)</f>
+        <v>41244.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>20</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
-        <v>192</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="5"/>
-        <v>28</v>
-      </c>
-      <c r="G17" s="8" t="str">
-        <f>CONCATENATE($A$31,$C$31,$A$32,$C$31,$A$33,$C$31,$A$34)</f>
+        <f>ROUNDUP(C17/6,0)</f>
+        <v>6</v>
+      </c>
+      <c r="E17" s="7" t="str">
+        <f>CONCATENATE($A$31,$B$35,$A$32,$B$35,$A$33,$B$35,$A$34)</f>
         <v>951926, 1024072, 1001231, 1028907</v>
       </c>
-      <c r="H17" s="9">
-        <v>5</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="2"/>
-        <v>120</v>
-      </c>
-      <c r="J17" s="3">
-        <f t="shared" si="3"/>
-        <v>41254</v>
-      </c>
-      <c r="K17" s="3">
-        <f t="shared" si="4"/>
-        <v>41257</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>30</v>
+      </c>
+      <c r="G17" s="3">
+        <f>B17+(F17/24)+$A$22</f>
+        <v>41250.25</v>
+      </c>
+      <c r="H17" s="3">
+        <f>$A$22+B17+(C17/24)</f>
+        <v>41250.333333333336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>21</v>
       </c>
       <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <f>ROUNDUP(C18/6,0)</f>
         <v>2</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="E18">
-        <f>SUM(B18:C18)</f>
-        <v>23</v>
-      </c>
-      <c r="G18" t="str">
+      <c r="E18" t="str">
         <f>CONCATENATE($A$34)</f>
         <v>1028907</v>
       </c>
-      <c r="H18" s="9">
-        <v>2</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-      <c r="J18" s="3">
-        <f t="shared" si="3"/>
-        <v>41252</v>
-      </c>
-      <c r="K18" s="3">
-        <f t="shared" si="4"/>
-        <v>41252</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>12</v>
+      </c>
+      <c r="G18" s="3">
+        <f>B18+(F18/24)+$A$22</f>
+        <v>41250.5</v>
+      </c>
+      <c r="H18" s="3">
+        <f>$A$22+B18+(C18/24)</f>
+        <v>41250.333333333336</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>41229</v>
       </c>
@@ -1676,24 +1516,16 @@
         <f>B22-A22</f>
         <v>20</v>
       </c>
-      <c r="E22">
-        <f>MAX(E2:E16)</f>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>41281</v>
       </c>
@@ -1702,44 +1534,42 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>951926</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>1024072</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>1001231</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
-      </c>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>1028907</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
-      </c>
-      <c r="E34" s="6"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1751,8 +1581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added student IDs to gantt chart and log sheet
</commit_message>
<xml_diff>
--- a/docs/logs/Gantt_chart.xlsx
+++ b/docs/logs/Gantt_chart.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Start Day</t>
+  </si>
+  <si>
+    <t>951926, 1024072, 1001231, 1028907</t>
   </si>
 </sst>
 </file>
@@ -390,6 +393,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -521,11 +529,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="100258944"/>
-        <c:axId val="100260864"/>
+        <c:axId val="102823040"/>
+        <c:axId val="102824960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="100258944"/>
+        <c:axId val="102823040"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -559,7 +567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100260864"/>
+        <c:crossAx val="102824960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -567,7 +575,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100260864"/>
+        <c:axId val="102824960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -599,7 +607,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="100258944"/>
+        <c:crossAx val="102823040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -623,13 +631,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>189941</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>571499</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -943,7 +951,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,7 +1003,7 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <f>ROUNDUP(C2/6,0)</f>
+        <f t="shared" ref="D2:D18" si="0">ROUNDUP(C2/6,0)</f>
         <v>1</v>
       </c>
       <c r="E2" t="str">
@@ -1006,11 +1014,11 @@
         <v>2</v>
       </c>
       <c r="G2" s="3">
-        <f>B2+(F2/24)+$A$22</f>
+        <f t="shared" ref="G2:G18" si="1">B2+(F2/24)+$A$22</f>
         <v>41229.083333333336</v>
       </c>
       <c r="H2" s="3">
-        <f>$A$22+B2+(C2/24)</f>
+        <f t="shared" ref="H2:H18" si="2">$A$22+B2+(C2/24)</f>
         <v>41229.125</v>
       </c>
     </row>
@@ -1025,7 +1033,7 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <f>ROUNDUP(C3/6,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E3" t="str">
@@ -1036,11 +1044,11 @@
         <v>3</v>
       </c>
       <c r="G3" s="3">
-        <f>B3+(F3/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41229.125</v>
       </c>
       <c r="H3" s="3">
-        <f>$A$22+B3+(C3/24)</f>
+        <f t="shared" si="2"/>
         <v>41229.166666666664</v>
       </c>
     </row>
@@ -1055,7 +1063,7 @@
         <v>5</v>
       </c>
       <c r="D4">
-        <f>ROUNDUP(C4/6,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E4" t="str">
@@ -1066,11 +1074,11 @@
         <v>3</v>
       </c>
       <c r="G4" s="3">
-        <f>B4+(F4/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41230.125</v>
       </c>
       <c r="H4" s="3">
-        <f>$A$22+B4+(C4/24)</f>
+        <f t="shared" si="2"/>
         <v>41230.208333333336</v>
       </c>
     </row>
@@ -1085,7 +1093,7 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <f>ROUNDUP(C5/6,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E5" t="str">
@@ -1096,11 +1104,11 @@
         <v>1.5</v>
       </c>
       <c r="G5" s="3">
-        <f>B5+(F5/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41230.0625</v>
       </c>
       <c r="H5" s="3">
-        <f>$A$22+B5+(C5/24)</f>
+        <f t="shared" si="2"/>
         <v>41230.333333333336</v>
       </c>
     </row>
@@ -1115,7 +1123,7 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <f>ROUNDUP(C6/6,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E6" t="str">
@@ -1126,11 +1134,11 @@
         <v>6</v>
       </c>
       <c r="G6" s="3">
-        <f>B6+(F6/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41231.25</v>
       </c>
       <c r="H6" s="3">
-        <f>$A$22+B6+(C6/24)</f>
+        <f t="shared" si="2"/>
         <v>41231.5</v>
       </c>
     </row>
@@ -1145,7 +1153,7 @@
         <v>4</v>
       </c>
       <c r="D7">
-        <f>ROUNDUP(C7/6,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E7" t="str">
@@ -1156,11 +1164,11 @@
         <v>6</v>
       </c>
       <c r="G7" s="3">
-        <f>B7+(F7/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41233.25</v>
       </c>
       <c r="H7" s="3">
-        <f>$A$22+B7+(C7/24)</f>
+        <f t="shared" si="2"/>
         <v>41233.166666666664</v>
       </c>
     </row>
@@ -1175,7 +1183,7 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <f>ROUNDUP(C8/6,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E8" t="str">
@@ -1186,11 +1194,11 @@
         <v>3</v>
       </c>
       <c r="G8" s="3">
-        <f>B8+(F8/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41234.125</v>
       </c>
       <c r="H8" s="3">
-        <f>$A$22+B8+(C8/24)</f>
+        <f t="shared" si="2"/>
         <v>41234.083333333336</v>
       </c>
     </row>
@@ -1205,7 +1213,7 @@
         <v>4</v>
       </c>
       <c r="D9">
-        <f>ROUNDUP(C9/6,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E9" t="str">
@@ -1216,11 +1224,11 @@
         <v>1.5</v>
       </c>
       <c r="G9" s="3">
-        <f>B9+(F9/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41234.0625</v>
       </c>
       <c r="H9" s="3">
-        <f>$A$22+B9+(C9/24)</f>
+        <f t="shared" si="2"/>
         <v>41234.166666666664</v>
       </c>
     </row>
@@ -1235,7 +1243,7 @@
         <v>60</v>
       </c>
       <c r="D10">
-        <f>ROUNDUP(C10/6,0)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E10" t="str">
@@ -1246,11 +1254,11 @@
         <v>12</v>
       </c>
       <c r="G10" s="3">
-        <f>B10+(F10/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41235.5</v>
       </c>
       <c r="H10" s="3">
-        <f>$A$22+B10+(C10/24)</f>
+        <f t="shared" si="2"/>
         <v>41237.5</v>
       </c>
     </row>
@@ -1265,7 +1273,7 @@
         <v>16</v>
       </c>
       <c r="D11">
-        <f>ROUNDUP(C11/6,0)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E11" t="str">
@@ -1276,11 +1284,11 @@
         <v>6</v>
       </c>
       <c r="G11" s="3">
-        <f>B11+(F11/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41238.25</v>
       </c>
       <c r="H11" s="3">
-        <f>$A$22+B11+(C11/24)</f>
+        <f t="shared" si="2"/>
         <v>41238.666666666664</v>
       </c>
     </row>
@@ -1295,7 +1303,7 @@
         <v>56</v>
       </c>
       <c r="D12">
-        <f>ROUNDUP(C12/6,0)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E12" t="str">
@@ -1306,11 +1314,11 @@
         <v>30</v>
       </c>
       <c r="G12" s="3">
-        <f>B12+(F12/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41236.25</v>
       </c>
       <c r="H12" s="3">
-        <f>$A$22+B12+(C12/24)</f>
+        <f t="shared" si="2"/>
         <v>41237.333333333336</v>
       </c>
     </row>
@@ -1325,7 +1333,7 @@
         <v>8</v>
       </c>
       <c r="D13">
-        <f>ROUNDUP(C13/6,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E13" t="str">
@@ -1336,11 +1344,11 @@
         <v>6</v>
       </c>
       <c r="G13" s="3">
-        <f>B13+(F13/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41242.25</v>
       </c>
       <c r="H13" s="3">
-        <f>$A$22+B13+(C13/24)</f>
+        <f t="shared" si="2"/>
         <v>41242.333333333336</v>
       </c>
     </row>
@@ -1355,7 +1363,7 @@
         <v>10</v>
       </c>
       <c r="D14">
-        <f>ROUNDUP(C14/6,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E14" t="str">
@@ -1366,11 +1374,11 @@
         <v>6</v>
       </c>
       <c r="G14" s="3">
-        <f>B14+(F14/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41244.25</v>
       </c>
       <c r="H14" s="3">
-        <f>$A$22+B14+(C14/24)</f>
+        <f t="shared" si="2"/>
         <v>41244.416666666664</v>
       </c>
     </row>
@@ -1385,7 +1393,7 @@
         <v>6</v>
       </c>
       <c r="D15">
-        <f>ROUNDUP(C15/6,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E15" t="str">
@@ -1396,11 +1404,11 @@
         <v>0.5</v>
       </c>
       <c r="G15" s="3">
-        <f>B15+(F15/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41245.020833333336</v>
       </c>
       <c r="H15" s="3">
-        <f>$A$22+B15+(C15/24)</f>
+        <f t="shared" si="2"/>
         <v>41245.25</v>
       </c>
     </row>
@@ -1415,7 +1423,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="5">
-        <f>ROUNDUP(C16/6,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E16" s="5" t="str">
@@ -1426,11 +1434,11 @@
         <v>18</v>
       </c>
       <c r="G16" s="8">
-        <f>B16+(F16/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41244.75</v>
       </c>
       <c r="H16" s="8">
-        <f>$A$22+B16+(C16/24)</f>
+        <f t="shared" si="2"/>
         <v>41244.5</v>
       </c>
     </row>
@@ -1445,7 +1453,7 @@
         <v>32</v>
       </c>
       <c r="D17">
-        <f>ROUNDUP(C17/6,0)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E17" s="7" t="str">
@@ -1456,11 +1464,11 @@
         <v>30</v>
       </c>
       <c r="G17" s="3">
-        <f>B17+(F17/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41250.25</v>
       </c>
       <c r="H17" s="3">
-        <f>$A$22+B17+(C17/24)</f>
+        <f t="shared" si="2"/>
         <v>41250.333333333336</v>
       </c>
     </row>
@@ -1475,7 +1483,7 @@
         <v>8</v>
       </c>
       <c r="D18">
-        <f>ROUNDUP(C18/6,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E18" t="str">
@@ -1486,11 +1494,11 @@
         <v>12</v>
       </c>
       <c r="G18" s="3">
-        <f>B18+(F18/24)+$A$22</f>
+        <f t="shared" si="1"/>
         <v>41250.5</v>
       </c>
       <c r="H18" s="3">
-        <f>$A$22+B18+(C18/24)</f>
+        <f t="shared" si="2"/>
         <v>41250.333333333336</v>
       </c>
     </row>
@@ -1579,14 +1587,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>